<commit_message>
feat: export csharp file.
</commit_message>
<xml_diff>
--- a/sheets/Job.xlsx
+++ b/sheets/Job.xlsx
@@ -9,67 +9,59 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
-  <si>
-    <t xml:space="preserve">Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HeadPic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JobPic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrefabName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dodge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Res</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UsedPhyAttackIds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UsedSkillIds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+  <si>
+    <t xml:space="preserve">id#number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">head_pic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">job_pic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prefab_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attack#number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">defense#number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hit#number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dodge#number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cri#number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res#number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">used_phy_attack_ids#number[]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">used_skill_ids#number[]</t>
   </si>
   <si>
     <t xml:space="preserve">编号</t>
@@ -126,10 +118,10 @@
     <t xml:space="preserve">暴击 刺客</t>
   </si>
   <si>
-    <t xml:space="preserve">101;102;103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">104;105;106;107;108;109</t>
+    <t xml:space="preserve">101,102,103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">104,105,106,107,108,109</t>
   </si>
   <si>
     <t xml:space="preserve">战士</t>
@@ -172,8 +164,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -181,7 +174,6 @@
       <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="0"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
@@ -255,7 +247,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -270,6 +262,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -289,12 +289,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="K30" activeCellId="0" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.96484375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -314,7 +314,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="33.25"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -358,7 +358,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -366,108 +366,106 @@
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>150</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>150</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>100</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>100</v>
@@ -476,40 +474,36 @@
         <v>100</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>150</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>100</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>100</v>
@@ -518,36 +512,36 @@
         <v>100</v>
       </c>
       <c r="K5" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="L5" s="2" t="n">
         <v>200</v>
-      </c>
-      <c r="L5" s="2" t="n">
-        <v>100</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>100</v>
@@ -556,52 +550,19 @@
         <v>100</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>120</v>
-      </c>
-      <c r="H7" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="J7" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>80</v>
-      </c>
-      <c r="L7" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
+    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D23" s="5"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -611,50 +572,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.96484375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.96484375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>